<commit_message>
Add education test added (with excel file)
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginList.xlsx
+++ b/src/test/resources/LoginList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihsan\IdeaProjects\Batch5Mentor_IA\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihsan\IdeaProjects\Batch5_Mentor_Cucumber_IA\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FD0F32-B00D-457B-8B17-AB1DAE52F2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D091013A-B499-4A38-9AC0-A988A2EA6EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27405" yWindow="1395" windowWidth="21600" windowHeight="11235" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="116">
   <si>
     <t>Your Name</t>
   </si>
@@ -105,9 +105,6 @@
     <t>fromdate</t>
   </si>
   <si>
-    <t>Todate</t>
-  </si>
-  <si>
     <t>Program Desc</t>
   </si>
   <si>
@@ -328,6 +325,57 @@
   </si>
   <si>
     <t>User4461</t>
+  </si>
+  <si>
+    <t>11/01/2002</t>
+  </si>
+  <si>
+    <t>12/12/2005</t>
+  </si>
+  <si>
+    <t>11/01/2003</t>
+  </si>
+  <si>
+    <t>12/12/2006</t>
+  </si>
+  <si>
+    <t>11/01/2004</t>
+  </si>
+  <si>
+    <t>12/12/2007</t>
+  </si>
+  <si>
+    <t>11/01/2005</t>
+  </si>
+  <si>
+    <t>12/12/2008</t>
+  </si>
+  <si>
+    <t>11/01/2006</t>
+  </si>
+  <si>
+    <t>12/12/2009</t>
+  </si>
+  <si>
+    <t>11/01/2007</t>
+  </si>
+  <si>
+    <t>12/12/2010</t>
+  </si>
+  <si>
+    <t>11/01/2008</t>
+  </si>
+  <si>
+    <t>12/12/2011</t>
+  </si>
+  <si>
+    <t>11/01/2009</t>
+  </si>
+  <si>
+    <t>12/12/2012</t>
+  </si>
+  <si>
+    <t>ToDate</t>
   </si>
 </sst>
 </file>
@@ -409,13 +457,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -713,206 +762,206 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
       </c>
       <c r="D3">
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
       </c>
       <c r="D4">
         <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>62</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
       </c>
       <c r="D5">
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
       </c>
       <c r="D6">
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
         <v>67</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>68</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
       </c>
       <c r="D7">
         <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>71</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
       </c>
       <c r="D8">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
         <v>73</v>
       </c>
-      <c r="B9" t="s">
-        <v>74</v>
-      </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9">
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
         <v>75</v>
       </c>
-      <c r="B10" t="s">
-        <v>76</v>
-      </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
         <v>77</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>78</v>
-      </c>
-      <c r="C11" t="s">
-        <v>79</v>
       </c>
       <c r="D11">
         <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
         <v>80</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>81</v>
-      </c>
-      <c r="C12" t="s">
-        <v>82</v>
       </c>
       <c r="D12">
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -925,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1016,7 +1065,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>17</v>
@@ -1038,13 +1087,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1188,24 +1237,24 @@
     </row>
     <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1226,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D8DB64-3C2D-4923-B33A-9078A63670CF}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1235,8 +1284,8 @@
     <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
     <col min="9" max="9" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1251,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>22</v>
@@ -1263,10 +1312,10 @@
         <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1280,22 +1329,22 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2">
-        <v>11122021</v>
-      </c>
-      <c r="H2">
-        <v>12122022</v>
+        <v>38</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1309,22 +1358,22 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3">
-        <v>11122020</v>
-      </c>
-      <c r="H3">
-        <v>12122022</v>
+        <v>39</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1338,22 +1387,22 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4">
-        <v>11122019</v>
-      </c>
-      <c r="H4">
-        <v>12122022</v>
+        <v>40</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1367,22 +1416,22 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5">
-        <v>11122021</v>
-      </c>
-      <c r="H5">
-        <v>12122022</v>
+        <v>38</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1396,22 +1445,22 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6">
-        <v>11122020</v>
-      </c>
-      <c r="H6">
-        <v>12122022</v>
+        <v>39</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1425,22 +1474,22 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7">
-        <v>11122019</v>
-      </c>
-      <c r="H7">
-        <v>12122022</v>
+        <v>40</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1454,22 +1503,22 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8">
-        <v>11122021</v>
-      </c>
-      <c r="H8">
-        <v>12122022</v>
+        <v>38</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1483,22 +1532,22 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9">
-        <v>11122020</v>
-      </c>
-      <c r="H9">
-        <v>12122022</v>
+        <v>39</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="I9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -1512,25 +1561,26 @@
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10">
-        <v>11122019</v>
-      </c>
-      <c r="H10">
-        <v>12122022</v>
+        <v>40</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7C752E4A-B9C6-485B-BA33-A742D29E64AE}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{35C09A7B-D3D8-4A9C-A1BC-B50E0CB82EBB}"/>

</xml_diff>